<commit_message>
#237-Enhanced Sales Agent Collection Summary Report
</commit_message>
<xml_diff>
--- a/Beelina.API/Templates/ReportTemplates/SalesAgentCollectionSummaryReport_Template.xlsx
+++ b/Beelina.API/Templates/ReportTemplates/SalesAgentCollectionSummaryReport_Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Beelina\Beelina.API\Templates\ReportTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49734D1D-FF0B-4B68-B1D7-43A9AE85025F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B54B3CE-9380-4BE5-8DA5-FD05057CFA09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0BCC69E0-6071-4C91-9E26-A9758A532CC5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Account Name</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>Bad Order</t>
+  </si>
+  <si>
+    <t>Collection Register</t>
   </si>
 </sst>
 </file>
@@ -66,7 +69,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,6 +85,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -91,7 +110,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -99,19 +118,74 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,46 +520,111 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36CBF8D9-8B47-4262-BED7-EC6F2F939521}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="3"/>
+    <col min="2" max="2" width="9.140625" style="1"/>
     <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B9" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C9" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D9" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E9" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F9" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G9" s="9" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A7:G7"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A5:G5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>